<commit_message>
Généré des requirements propres à P4_Cleaning_EDA, et à P4_Modelling | P4_Modelling 2 et 3 pour tester des choses sur le côté | Stockage des résultats des permutation_importance en pickles | Correction d'une grosse erreur dans CustTranformer (stratégies bloquées) et récupération des noms des features par le CustTransformer | Adaptation de plot_scv_multi_scores pour le RandomizedSearchCV | fonction qui trace le Regularization path | Classes 'ZscoreSampleFilter' et 'LOFSampleFilter' pour éliminer les outliers sur critères. | Score toujours sous 0.5 (sauvegarde avant filltrage des outliers en amont).
</commit_message>
<xml_diff>
--- a/perf_models.xlsx
+++ b/perf_models.xlsx
@@ -100,14 +100,14 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -297,11 +297,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="134454784"/>
-        <c:axId val="136577024"/>
+        <c:axId val="624181248"/>
+        <c:axId val="177944768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="134454784"/>
+        <c:axId val="624181248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -310,7 +310,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136577024"/>
+        <c:crossAx val="177944768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -318,7 +318,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136577024"/>
+        <c:axId val="177944768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -329,7 +329,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134454784"/>
+        <c:crossAx val="624181248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -704,26 +704,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
@@ -749,22 +749,22 @@
       <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>0.79</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>-10357232.18</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>-2905257.33</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>0.42</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>-16547287.32</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>-4814982.34</v>
       </c>
     </row>
@@ -772,22 +772,22 @@
       <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>0.15</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>-20925186.440000001</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>-5981888.7300000004</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>0.13</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>-19768711.960000001</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>-6064050.5899999999</v>
       </c>
     </row>
@@ -795,22 +795,22 @@
       <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>0.17</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>-20726359.050000001</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>-6090748.6200000001</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>0.12</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>-19997074.440000001</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>-6261315.3600000003</v>
       </c>
     </row>
@@ -818,22 +818,22 @@
       <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>0.1</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>-21490552.559999999</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>-6307190.0199999996</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>0.09</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>-20264437.02</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>-6277325.6900000004</v>
       </c>
     </row>
@@ -841,22 +841,22 @@
       <c r="C8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>0.83</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>-9267708.6600000001</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>-1876858.2</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>0.5</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>-15470638.359999999</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <v>-4405524.74</v>
       </c>
     </row>
@@ -864,22 +864,22 @@
       <c r="C9" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>0.96</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>-4201410.1100000003</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>-1529017.45</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>0.44</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>-16423255.43</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>-4435137.79</v>
       </c>
     </row>
@@ -887,46 +887,46 @@
       <c r="C10" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>0.9</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>-7171963.1699999999</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>-2041512.31</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <v>0.57999999999999996</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>-14125301.869999999</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <v>-4032296.15</v>
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1" t="s">
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D14" t="s">

</xml_diff>